<commit_message>
Sample fixed from 1998Jul28_Art3_TrapA_wk31 to 1998Jul29_Art3_TrapA_Wk31
</commit_message>
<xml_diff>
--- a/6_referenceseqs_metadata/PlatesEF_metadata/Samples_for_sequencing_Zack_collection_Nov_2016_DY_TH_17_Feb_2017.xlsx
+++ b/6_referenceseqs_metadata/PlatesEF_metadata/Samples_for_sequencing_Zack_collection_Nov_2016_DY_TH_17_Feb_2017.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Dropbox/Working_docs/Roslin_Greenland/2017/bulk_samples/ArcDyn_scripts/6_referenceseqs_metadata/PlatesEF_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD08F03-AA55-FE45-BD4F-312A177FED1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF934260-DD0F-C442-ABAA-7C437E306DD1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7940" yWindow="1560" windowWidth="33600" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="edited" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="107" r:id="rId4"/>
+    <pivotCache cacheId="133" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -49,10 +49,29 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={9479B03A-1BC2-414B-8BB1-1531CEB2BF52}</author>
+    <author>tc={BB42D55A-EFF7-3046-AE2D-90EDF0135273}</author>
     <author>dy</author>
   </authors>
   <commentList>
-    <comment ref="E125" authorId="0" shapeId="0" xr:uid="{EEC82009-59AA-F64C-80EE-0F5F089F6E86}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{9479B03A-1BC2-414B-8BB1-1531CEB2BF52}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    originally, 1998Jul28_Art3_TrapA_wk31, but there are no Jul28 samples, only Jul29 samples. 
+So i changed to 1998Jul29_Art3_TrapA_Wk31</t>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="1" shapeId="0" xr:uid="{BB42D55A-EFF7-3046-AE2D-90EDF0135273}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    this sample is part of PlatesAB but there is no sample in PlatesAB, so this is an original sample (a make up sample)</t>
+      </text>
+    </comment>
+    <comment ref="E125" authorId="2" shapeId="0" xr:uid="{EEC82009-59AA-F64C-80EE-0F5F089F6E86}">
       <text>
         <r>
           <rPr>
@@ -90,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3704" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3704" uniqueCount="722">
   <si>
     <t>98_B_30</t>
   </si>
@@ -2253,6 +2272,9 @@
   </si>
   <si>
     <t>ME200_2</t>
+  </si>
+  <si>
+    <t>1998Jul29_Art3_TrapA_Wk31</t>
   </si>
 </sst>
 </file>
@@ -2354,6 +2376,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Douglas Yu (BIO - Staff)" id="{92C4DC3C-B106-3342-A3A3-CA109E108F79}" userId="S::b042@uea.ac.uk::5608b1c6-a62d-49b6-952d-1b3572938aae" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6269,7 +6297,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{224243D3-B9EE-A447-B668-A741793EB114}" name="PivotTable1" cacheId="107" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{224243D3-B9EE-A447-B668-A741793EB114}" name="PivotTable1" cacheId="133" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B196" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" dataField="1" showAll="0" sortType="ascending">
@@ -7349,13 +7377,25 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A3" dT="2019-01-24T14:52:03.97" personId="{92C4DC3C-B106-3342-A3A3-CA109E108F79}" id="{9479B03A-1BC2-414B-8BB1-1531CEB2BF52}">
+    <text>originally, 1998Jul28_Art3_TrapA_wk31, but there are no Jul28 samples, only Jul29 samples. 
+So i changed to 1998Jul29_Art3_TrapA_Wk31</text>
+  </threadedComment>
+  <threadedComment ref="A4" dT="2019-01-24T15:26:41.27" personId="{92C4DC3C-B106-3342-A3A3-CA109E108F79}" id="{BB42D55A-EFF7-3046-AE2D-90EDF0135273}">
+    <text>this sample is part of PlatesAB but there is no sample in PlatesAB, so this is an original sample (a make up sample)</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1460C49D-40E3-1348-B1B6-B637B39D6C3C}">
   <dimension ref="A1:Q200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7480,7 +7520,7 @@
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>700</v>
+        <v>721</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>

</xml_diff>